<commit_message>
modefied the standarized and cleaned cw T0 data template for na screening and creating new standardized and cleaned templates for cw T1 data
</commit_message>
<xml_diff>
--- a/data/cleaned/cleaned_data_for_nascreening_analysis/alraune_template/cw_T0_BTEXN.xlsx
+++ b/data/cleaned/cleaned_data_for_nascreening_analysis/alraune_template/cw_T0_BTEXN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\preprocessed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\cleaned\cleaned_data_for_nascreening_analysis\alraune_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAC31E2-0039-4FE4-B9E7-900AF508DAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598FC896-7CBC-4FD3-81BA-F03F883D6E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contaminants" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="209">
-  <si>
-    <t>-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="208">
   <si>
     <t>mg/l</t>
   </si>
@@ -972,7 +969,7 @@
   </sheetPr>
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -993,31 +990,31 @@
   <sheetData>
     <row r="1" spans="1:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="C1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1055,25 +1052,25 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1109,213 +1106,213 @@
     </row>
     <row r="3" spans="1:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="H3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="H5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="7">
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="7">
         <v>4</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="7">
         <v>3</v>
@@ -1333,166 +1330,166 @@
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>130</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="7">
         <v>3</v>
@@ -1507,79 +1504,79 @@
         <v>3</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="H18" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="I18" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="7">
         <v>2</v>
@@ -1594,47 +1591,47 @@
         <v>0</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
@@ -1652,47 +1649,47 @@
         <v>0</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="I22" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="7">
         <v>7</v>
@@ -1701,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F23" s="7">
         <v>0</v>
@@ -1710,47 +1707,47 @@
         <v>0</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="I24" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" t="s">
         <v>188</v>
-      </c>
-      <c r="B25" t="s">
-        <v>189</v>
       </c>
       <c r="C25" s="6">
         <v>0</v>
@@ -1788,8 +1785,8 @@
   </sheetPr>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1799,94 +1796,92 @@
   <sheetData>
     <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>201</v>
       </c>
-      <c r="H1" t="s">
-        <v>202</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -1901,36 +1896,36 @@
         <v>-83</v>
       </c>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
       <c r="I3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1945,13 +1940,13 @@
         <v>-138</v>
       </c>
       <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
       <c r="I4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -1971,10 +1966,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -1989,36 +1984,36 @@
         <v>-132.5</v>
       </c>
       <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
       <c r="I5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -2033,13 +2028,13 @@
         <v>-134</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J6" s="7">
         <v>0</v>
@@ -2059,10 +2054,10 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -2077,36 +2072,36 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -2121,13 +2116,13 @@
         <v>-166</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" s="7">
         <v>0</v>
@@ -2147,10 +2142,10 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -2165,13 +2160,13 @@
         <v>-192</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J9" s="7">
         <v>0</v>
@@ -2186,15 +2181,15 @@
         <v>0</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -2209,13 +2204,13 @@
         <v>-133</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="7">
         <v>0</v>
@@ -2235,10 +2230,10 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -2253,13 +2248,13 @@
         <v>-183.2</v>
       </c>
       <c r="G11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="7">
         <v>0</v>
@@ -2274,15 +2269,15 @@
         <v>0</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -2297,13 +2292,13 @@
         <v>-132</v>
       </c>
       <c r="G12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J12" s="7">
         <v>0</v>
@@ -2318,15 +2313,15 @@
         <v>0</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6">
         <v>0</v>
@@ -2347,7 +2342,7 @@
         <v>3.7</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J13" s="7">
         <v>0</v>
@@ -2362,15 +2357,15 @@
         <v>0</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
@@ -2385,13 +2380,13 @@
         <v>-118</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J14" s="7">
         <v>0</v>
@@ -2406,15 +2401,15 @@
         <v>0</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6">
         <v>0</v>
@@ -2429,13 +2424,13 @@
         <v>-164</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" s="7">
         <v>0</v>
@@ -2450,15 +2445,15 @@
         <v>0</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -2473,13 +2468,13 @@
         <v>-132</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="7">
         <v>0</v>
@@ -2499,10 +2494,10 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
@@ -2517,13 +2512,13 @@
         <v>-128</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17" s="7">
         <v>0</v>
@@ -2538,15 +2533,15 @@
         <v>0</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="6">
         <v>0</v>
@@ -2561,13 +2556,13 @@
         <v>-141</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J18" s="7">
         <v>0</v>
@@ -2582,15 +2577,15 @@
         <v>0</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
@@ -2605,13 +2600,13 @@
         <v>-131</v>
       </c>
       <c r="G19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J19" s="7">
         <v>0</v>
@@ -2631,10 +2626,10 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="6">
         <v>0</v>
@@ -2646,13 +2641,13 @@
         <v>-109</v>
       </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J20" s="7">
         <v>0</v>
@@ -2667,15 +2662,15 @@
         <v>0</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="6">
         <v>0</v>
@@ -2690,13 +2685,13 @@
         <v>-159</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" s="7">
         <v>0</v>
@@ -2711,15 +2706,15 @@
         <v>0</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="6">
         <v>0</v>
@@ -2734,36 +2729,36 @@
         <v>-163</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I22" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="J22" s="7">
-        <v>0</v>
-      </c>
-      <c r="K22" s="7">
-        <v>0</v>
-      </c>
-      <c r="L22" s="7">
-        <v>0</v>
-      </c>
-      <c r="M22" s="7">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6">
         <v>0</v>
@@ -2778,13 +2773,13 @@
         <v>-117</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23" s="7">
         <v>0</v>
@@ -2804,10 +2799,10 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="6">
         <v>0</v>
@@ -2822,13 +2817,13 @@
         <v>-132</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J24" s="7">
         <v>0</v>
@@ -2843,15 +2838,15 @@
         <v>0</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" t="s">
         <v>188</v>
-      </c>
-      <c r="B25" t="s">
-        <v>189</v>
       </c>
       <c r="C25" s="6">
         <v>0</v>
@@ -2866,10 +2861,10 @@
         <v>-101</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I25" s="6">
         <v>0</v>

</xml_diff>